<commit_message>
import pictures for XLSX
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/picture.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/picture.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19155" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19155" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,14 +61,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -87,7 +87,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="600075" y="180975"/>
+          <a:off x="419100" y="180975"/>
           <a:ext cx="4286250" cy="3048000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -181,19 +181,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>169332</xdr:colOff>
+      <xdr:colOff>152399</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>60127</xdr:rowOff>
+      <xdr:rowOff>108941</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
+      <xdr:colOff>504824</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>154780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="black-wallpaper.gif"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="rainbow.gif"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -206,8 +206,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6265332" y="822127"/>
-          <a:ext cx="5650442" cy="3178374"/>
+          <a:off x="6248399" y="870941"/>
+          <a:ext cx="5838825" cy="3284339"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>

</xml_diff>